<commit_message>
risultati suplin e quad di 16 e 79
</commit_message>
<xml_diff>
--- a/F16_truncated/results_f16_quad.xlsx
+++ b/F16_truncated/results_f16_quad.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView activeTab="0"/>
@@ -12,6 +12,10 @@
     <sheet name="time_4" sheetId="5" r:id="rId7"/>
     <sheet name="niter_4" sheetId="6" r:id="rId8"/>
     <sheet name="f_val_4" sheetId="7" r:id="rId9"/>
+    <sheet name="time5" sheetId="8" r:id="rId10"/>
+    <sheet name="niter_5" sheetId="9" r:id="rId11"/>
+    <sheet name="f_val_5" sheetId="10" r:id="rId12"/>
+    <sheet name="ExactComparison" sheetId="11" r:id="rId13"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
@@ -19,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="60" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
   <si>
     <t>Row</t>
   </si>
@@ -49,12 +53,273 @@
   </si>
   <si>
     <t>Exact</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>FD1</t>
+  </si>
+  <si>
+    <t>FD2</t>
+  </si>
+  <si>
+    <t>h=1e-2</t>
+  </si>
+  <si>
+    <t>h=1e-4</t>
+  </si>
+  <si>
+    <t>h=1e-6</t>
+  </si>
+  <si>
+    <t>h=1e-8</t>
+  </si>
+  <si>
+    <t>h=1e-10</t>
+  </si>
+  <si>
+    <t>h=1e-12</t>
+  </si>
+  <si>
+    <t>Exact</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>FD1</t>
+  </si>
+  <si>
+    <t>FD2</t>
+  </si>
+  <si>
+    <t>h=1e-2</t>
+  </si>
+  <si>
+    <t>h=1e-4</t>
+  </si>
+  <si>
+    <t>h=1e-6</t>
+  </si>
+  <si>
+    <t>h=1e-8</t>
+  </si>
+  <si>
+    <t>h=1e-10</t>
+  </si>
+  <si>
+    <t>h=1e-12</t>
+  </si>
+  <si>
+    <t>Exact</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>FD1</t>
+  </si>
+  <si>
+    <t>FD2</t>
+  </si>
+  <si>
+    <t>h=1e-2</t>
+  </si>
+  <si>
+    <t>h=1e-4</t>
+  </si>
+  <si>
+    <t>h=1e-6</t>
+  </si>
+  <si>
+    <t>h=1e-8</t>
+  </si>
+  <si>
+    <t>h=1e-10</t>
+  </si>
+  <si>
+    <t>h=1e-12</t>
+  </si>
+  <si>
+    <t>Exact</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>FD1</t>
+  </si>
+  <si>
+    <t>FD2</t>
+  </si>
+  <si>
+    <t>h=1e-2</t>
+  </si>
+  <si>
+    <t>h=1e-4</t>
+  </si>
+  <si>
+    <t>h=1e-6</t>
+  </si>
+  <si>
+    <t>h=1e-8</t>
+  </si>
+  <si>
+    <t>h=1e-10</t>
+  </si>
+  <si>
+    <t>h=1e-12</t>
+  </si>
+  <si>
+    <t>Exact</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>FD1</t>
+  </si>
+  <si>
+    <t>FD2</t>
+  </si>
+  <si>
+    <t>h=1e-2</t>
+  </si>
+  <si>
+    <t>h=1e-4</t>
+  </si>
+  <si>
+    <t>h=1e-6</t>
+  </si>
+  <si>
+    <t>h=1e-8</t>
+  </si>
+  <si>
+    <t>h=1e-10</t>
+  </si>
+  <si>
+    <t>h=1e-12</t>
+  </si>
+  <si>
+    <t>Exact</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>FD1</t>
+  </si>
+  <si>
+    <t>FD2</t>
+  </si>
+  <si>
+    <t>h=1e-2</t>
+  </si>
+  <si>
+    <t>h=1e-4</t>
+  </si>
+  <si>
+    <t>h=1e-6</t>
+  </si>
+  <si>
+    <t>h=1e-8</t>
+  </si>
+  <si>
+    <t>h=1e-10</t>
+  </si>
+  <si>
+    <t>h=1e-12</t>
+  </si>
+  <si>
+    <t>Exact</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>FD1</t>
+  </si>
+  <si>
+    <t>FD2</t>
+  </si>
+  <si>
+    <t>h=1e-2</t>
+  </si>
+  <si>
+    <t>h=1e-4</t>
+  </si>
+  <si>
+    <t>h=1e-6</t>
+  </si>
+  <si>
+    <t>h=1e-8</t>
+  </si>
+  <si>
+    <t>h=1e-10</t>
+  </si>
+  <si>
+    <t>h=1e-12</t>
+  </si>
+  <si>
+    <t>Exact</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>FD1</t>
+  </si>
+  <si>
+    <t>FD2</t>
+  </si>
+  <si>
+    <t>h=1e-2</t>
+  </si>
+  <si>
+    <t>h=1e-4</t>
+  </si>
+  <si>
+    <t>h=1e-6</t>
+  </si>
+  <si>
+    <t>h=1e-8</t>
+  </si>
+  <si>
+    <t>h=1e-10</t>
+  </si>
+  <si>
+    <t>h=1e-12</t>
+  </si>
+  <si>
+    <t>Exact</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Avergae Time</t>
+  </si>
+  <si>
+    <t>Avergae Iter</t>
+  </si>
+  <si>
+    <t>Average fval</t>
+  </si>
+  <si>
+    <t>n=10^3</t>
+  </si>
+  <si>
+    <t>n=10^4</t>
+  </si>
+  <si>
+    <t>n=10^5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -69,7 +334,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -78,13 +343,31 @@
       <diagonal/>
     </border>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -92,22 +375,187 @@
 </styleSheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" customWidth="true"/>
-    <col min="2" max="2" width="10.5546875" customWidth="true"/>
-    <col min="3" max="3" width="13.5546875" customWidth="true"/>
-    <col min="4" max="4" width="10.5546875" customWidth="true"/>
-    <col min="5" max="5" width="10.5546875" customWidth="true"/>
-    <col min="6" max="6" width="10.5546875" customWidth="true"/>
-    <col min="7" max="7" width="9.5546875" customWidth="true"/>
-    <col min="8" max="8" width="10.5546875" customWidth="true"/>
+    <col min="1" max="1" width="4.82421875" customWidth="true"/>
+    <col min="2" max="2" width="12.37890625" customWidth="true"/>
+    <col min="3" max="3" width="12.37890625" customWidth="true"/>
+    <col min="4" max="4" width="12.37890625" customWidth="true"/>
+    <col min="5" max="5" width="12.37890625" customWidth="true"/>
+    <col min="6" max="6" width="12.37890625" customWidth="true"/>
+    <col min="7" max="7" width="12.37890625" customWidth="true"/>
+    <col min="8" max="8" width="12.37890625" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="0">
+        <v>-41443.758305751675</v>
+      </c>
+      <c r="C2" s="0">
+        <v>-41443.758305751522</v>
+      </c>
+      <c r="D2" s="0">
+        <v>-41443.758305751653</v>
+      </c>
+      <c r="E2" s="0">
+        <v>-41443.758305751573</v>
+      </c>
+      <c r="F2" s="0">
+        <v>-41443.758305751573</v>
+      </c>
+      <c r="G2" s="0">
+        <v>-41443.758305751573</v>
+      </c>
+      <c r="H2" s="0">
+        <v>-41443.758305751573</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="0">
+        <v>-41443.758305751289</v>
+      </c>
+      <c r="C3" s="0">
+        <v>-41443.758305751631</v>
+      </c>
+      <c r="D3" s="0">
+        <v>-41443.758305751624</v>
+      </c>
+      <c r="E3" s="0">
+        <v>-41443.758305751595</v>
+      </c>
+      <c r="F3" s="0">
+        <v>-41443.758305751573</v>
+      </c>
+      <c r="G3" s="0">
+        <v>-41443.758305751573</v>
+      </c>
+      <c r="H3" s="0">
+        <v>-41443.758305751573</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.15625" customWidth="true"/>
+    <col min="2" max="2" width="10.7109375" customWidth="true"/>
+    <col min="3" max="3" width="12.7109375" customWidth="true"/>
+    <col min="4" max="4" width="11.7109375" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="0">
+        <v>0.0094000400000000001</v>
+      </c>
+      <c r="C2" s="0">
+        <v>0.11551818888888891</v>
+      </c>
+      <c r="D2" s="0">
+        <v>10.731593818181819</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="0">
+        <v>20.800000000000001</v>
+      </c>
+      <c r="C3" s="0">
+        <v>29.555555555555557</v>
+      </c>
+      <c r="D3" s="0">
+        <v>112.63636363636364</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" s="0">
+        <v>-427.40447637484976</v>
+      </c>
+      <c r="C4" s="0">
+        <v>-4159.9324479061488</v>
+      </c>
+      <c r="D4" s="0">
+        <v>-41443.758305751573</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="4.82421875" customWidth="true"/>
+    <col min="2" max="2" width="10.7109375" customWidth="true"/>
+    <col min="3" max="3" width="14.7109375" customWidth="true"/>
+    <col min="4" max="4" width="9.7109375" customWidth="true"/>
+    <col min="5" max="5" width="10.7109375" customWidth="true"/>
+    <col min="6" max="6" width="10.7109375" customWidth="true"/>
+    <col min="7" max="7" width="10.7109375" customWidth="true"/>
+    <col min="8" max="8" width="10.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -141,25 +589,25 @@
         <v>1</v>
       </c>
       <c r="B2" s="0">
-        <v>0.032448560000000001</v>
+        <v>0.0067259799999999995</v>
       </c>
       <c r="C2" s="0">
-        <v>0.033317354545454543</v>
+        <v>0.0060835666666666658</v>
       </c>
       <c r="D2" s="0">
-        <v>0.028804649999999998</v>
+        <v>0.0066792999999999991</v>
       </c>
       <c r="E2" s="0">
-        <v>0.029720309999999993</v>
+        <v>0.0061341599999999996</v>
       </c>
       <c r="F2" s="0">
-        <v>0.031996330000000003</v>
+        <v>0.0059495699999999995</v>
       </c>
       <c r="G2" s="0">
-        <v>0.029882399999999996</v>
+        <v>0.0058839099999999991</v>
       </c>
       <c r="H2" s="0">
-        <v>0.038581440000000002</v>
+        <v>0.0094000400000000001</v>
       </c>
     </row>
     <row r="3">
@@ -167,25 +615,25 @@
         <v>2</v>
       </c>
       <c r="B3" s="0">
-        <v>0.22969701818181817</v>
+        <v>0.031168924999999997</v>
       </c>
       <c r="C3" s="0">
-        <v>0.22362271111111109</v>
+        <v>0.03089165</v>
       </c>
       <c r="D3" s="0">
-        <v>0.20024420999999998</v>
+        <v>0.029333540000000002</v>
       </c>
       <c r="E3" s="0">
-        <v>0.19315055454545457</v>
+        <v>0.029687700000000001</v>
       </c>
       <c r="F3" s="0">
-        <v>0.20718424999999999</v>
+        <v>0.030065970000000004</v>
       </c>
       <c r="G3" s="0">
-        <v>0.19948653999999999</v>
+        <v>0.02998785</v>
       </c>
       <c r="H3" s="0">
-        <v>0.038581440000000002</v>
+        <v>0.0094000400000000001</v>
       </c>
     </row>
   </sheetData>
@@ -193,99 +641,96 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" customWidth="true"/>
-    <col min="2" max="2" width="6.6640625" customWidth="true"/>
-    <col min="3" max="3" width="11.5546875" customWidth="true"/>
-    <col min="4" max="4" width="6.6640625" customWidth="true"/>
-    <col min="5" max="5" width="6.6640625" customWidth="true"/>
-    <col min="6" max="6" width="7.6640625" customWidth="true"/>
-    <col min="7" max="7" width="7.6640625" customWidth="true"/>
-    <col min="8" max="8" width="5.44140625" customWidth="true"/>
+    <col min="1" max="1" width="4.82421875" customWidth="true"/>
+    <col min="2" max="2" width="6.82421875" customWidth="true"/>
+    <col min="3" max="3" width="11.7109375" customWidth="true"/>
+    <col min="4" max="4" width="6.82421875" customWidth="true"/>
+    <col min="5" max="5" width="6.82421875" customWidth="true"/>
+    <col min="6" max="6" width="7.82421875" customWidth="true"/>
+    <col min="7" max="7" width="7.82421875" customWidth="true"/>
+    <col min="8" max="8" width="5.6015625" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B2" s="0">
-        <v>20.199999999999999</v>
+        <v>20.600000000000001</v>
       </c>
       <c r="C2" s="0">
-        <v>20.454545454545453</v>
+        <v>20.444444444444443</v>
       </c>
       <c r="D2" s="0">
-        <v>20.5</v>
+        <v>21</v>
       </c>
       <c r="E2" s="0">
-        <v>20.600000000000001</v>
+        <v>20.800000000000001</v>
       </c>
       <c r="F2" s="0">
-        <v>20.600000000000001</v>
+        <v>20.800000000000001</v>
       </c>
       <c r="G2" s="0">
-        <v>20.600000000000001</v>
+        <v>20.800000000000001</v>
       </c>
       <c r="H2" s="0">
-        <v>20.600000000000001</v>
+        <v>20.800000000000001</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B3" s="0">
-        <v>20.454545454545453</v>
+        <v>20.375</v>
       </c>
       <c r="C3" s="0">
-        <v>20.666666666666668</v>
+        <v>20.899999999999999</v>
       </c>
       <c r="D3" s="0">
-        <v>20.100000000000001</v>
+        <v>20.300000000000001</v>
       </c>
       <c r="E3" s="0">
-        <v>20.727272727272727</v>
+        <v>20.5</v>
       </c>
       <c r="F3" s="0">
-        <v>20.600000000000001</v>
+        <v>20.800000000000001</v>
       </c>
       <c r="G3" s="0">
-        <v>20.600000000000001</v>
+        <v>20.800000000000001</v>
       </c>
       <c r="H3" s="0">
-        <v>20.600000000000001</v>
+        <v>20.800000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -293,99 +738,96 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" customWidth="true"/>
-    <col min="2" max="2" width="12.21875" customWidth="true"/>
-    <col min="3" max="3" width="12.21875" customWidth="true"/>
-    <col min="4" max="4" width="12.21875" customWidth="true"/>
-    <col min="5" max="5" width="12.21875" customWidth="true"/>
-    <col min="6" max="6" width="12.21875" customWidth="true"/>
-    <col min="7" max="7" width="12.21875" customWidth="true"/>
-    <col min="8" max="8" width="12.21875" customWidth="true"/>
+    <col min="1" max="1" width="4.82421875" customWidth="true"/>
+    <col min="2" max="2" width="12.37890625" customWidth="true"/>
+    <col min="3" max="3" width="12.37890625" customWidth="true"/>
+    <col min="4" max="4" width="12.37890625" customWidth="true"/>
+    <col min="5" max="5" width="12.37890625" customWidth="true"/>
+    <col min="6" max="6" width="12.37890625" customWidth="true"/>
+    <col min="7" max="7" width="12.37890625" customWidth="true"/>
+    <col min="8" max="8" width="12.37890625" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B2" s="0">
-        <v>-427.40447637484931</v>
+        <v>-427.4044763748492</v>
       </c>
       <c r="C2" s="0">
-        <v>-427.40447637484982</v>
+        <v>-427.40447637484971</v>
       </c>
       <c r="D2" s="0">
+        <v>-427.40447637484942</v>
+      </c>
+      <c r="E2" s="0">
         <v>-427.40447637484976</v>
       </c>
-      <c r="E2" s="0">
-        <v>-427.40447637484959</v>
-      </c>
       <c r="F2" s="0">
-        <v>-427.40447637484959</v>
+        <v>-427.40447637484976</v>
       </c>
       <c r="G2" s="0">
-        <v>-427.40447637484959</v>
+        <v>-427.40447637484976</v>
       </c>
       <c r="H2" s="0">
-        <v>-427.40447637484959</v>
+        <v>-427.40447637484976</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="B3" s="0">
-        <v>-427.40447637484942</v>
+        <v>-427.40447637484931</v>
       </c>
       <c r="C3" s="0">
-        <v>-427.40447637484971</v>
+        <v>-427.40447637484993</v>
       </c>
       <c r="D3" s="0">
+        <v>-427.40447637484965</v>
+      </c>
+      <c r="E3" s="0">
         <v>-427.40447637484948</v>
       </c>
-      <c r="E3" s="0">
-        <v>-427.40447637484954</v>
-      </c>
       <c r="F3" s="0">
-        <v>-427.40447637484959</v>
+        <v>-427.40447637484976</v>
       </c>
       <c r="G3" s="0">
-        <v>-427.40447637484959</v>
+        <v>-427.40447637484976</v>
       </c>
       <c r="H3" s="0">
-        <v>-427.40447637484959</v>
+        <v>-427.40447637484976</v>
       </c>
     </row>
   </sheetData>
@@ -393,99 +835,96 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" customWidth="true"/>
-    <col min="2" max="2" width="12.5546875" customWidth="true"/>
-    <col min="3" max="3" width="10.5546875" customWidth="true"/>
-    <col min="4" max="4" width="12.5546875" customWidth="true"/>
-    <col min="5" max="5" width="9.5546875" customWidth="true"/>
-    <col min="6" max="6" width="12.5546875" customWidth="true"/>
-    <col min="7" max="7" width="12.5546875" customWidth="true"/>
-    <col min="8" max="8" width="12.5546875" customWidth="true"/>
+    <col min="1" max="1" width="4.82421875" customWidth="true"/>
+    <col min="2" max="2" width="12.7109375" customWidth="true"/>
+    <col min="3" max="3" width="9.7109375" customWidth="true"/>
+    <col min="4" max="4" width="12.7109375" customWidth="true"/>
+    <col min="5" max="5" width="12.7109375" customWidth="true"/>
+    <col min="6" max="6" width="12.7109375" customWidth="true"/>
+    <col min="7" max="7" width="12.7109375" customWidth="true"/>
+    <col min="8" max="8" width="12.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="B2" s="0">
-        <v>0.5018608714285715</v>
+        <v>0.16377944444444445</v>
       </c>
       <c r="C2" s="0">
-        <v>0.82075592000000008</v>
+        <v>0.10950169999999999</v>
       </c>
       <c r="D2" s="0">
-        <v>0.60324893333333329</v>
+        <v>0.11856961111111113</v>
       </c>
       <c r="E2" s="0">
-        <v>0.52524159999999998</v>
+        <v>0.1121470777777778</v>
       </c>
       <c r="F2" s="0">
-        <v>0.56137191111111118</v>
+        <v>0.11287488888888889</v>
       </c>
       <c r="G2" s="0">
-        <v>0.4821671666666667</v>
+        <v>0.11190612222222221</v>
       </c>
       <c r="H2" s="0">
-        <v>0.54519396666666675</v>
+        <v>0.11551818888888891</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="B3" s="0">
-        <v>3.4191590636363642</v>
+        <v>0.56362374999999998</v>
       </c>
       <c r="C3" s="0">
-        <v>3.0116439625</v>
+        <v>0.44899438750000004</v>
       </c>
       <c r="D3" s="0">
-        <v>3.0950700222222221</v>
+        <v>0.75795137000000001</v>
       </c>
       <c r="E3" s="0">
-        <v>2.9718068999999998</v>
+        <v>0.44807116666666669</v>
       </c>
       <c r="F3" s="0">
-        <v>2.9825360888888892</v>
+        <v>0.45212802222222215</v>
       </c>
       <c r="G3" s="0">
-        <v>3.0212218111111109</v>
+        <v>0.45149193333333326</v>
       </c>
       <c r="H3" s="0">
-        <v>0.54519396666666675</v>
+        <v>0.11551818888888891</v>
       </c>
     </row>
   </sheetData>
@@ -493,99 +932,96 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" customWidth="true"/>
-    <col min="2" max="2" width="11.5546875" customWidth="true"/>
-    <col min="3" max="3" width="6.6640625" customWidth="true"/>
-    <col min="4" max="4" width="11.5546875" customWidth="true"/>
-    <col min="5" max="5" width="11.5546875" customWidth="true"/>
-    <col min="6" max="6" width="11.5546875" customWidth="true"/>
-    <col min="7" max="7" width="11.5546875" customWidth="true"/>
-    <col min="8" max="8" width="11.5546875" customWidth="true"/>
+    <col min="1" max="1" width="4.82421875" customWidth="true"/>
+    <col min="2" max="2" width="11.7109375" customWidth="true"/>
+    <col min="3" max="3" width="11.7109375" customWidth="true"/>
+    <col min="4" max="4" width="11.7109375" customWidth="true"/>
+    <col min="5" max="5" width="11.7109375" customWidth="true"/>
+    <col min="6" max="6" width="11.7109375" customWidth="true"/>
+    <col min="7" max="7" width="11.7109375" customWidth="true"/>
+    <col min="8" max="8" width="11.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>3</v>
+        <v>43</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="B2" s="0">
-        <v>29.142857142857142</v>
+        <v>32.333333333333336</v>
       </c>
       <c r="C2" s="0">
-        <v>32.399999999999999</v>
+        <v>29.222222222222221</v>
       </c>
       <c r="D2" s="0">
-        <v>29.222222222222221</v>
+        <v>29.444444444444443</v>
       </c>
       <c r="E2" s="0">
-        <v>29.777777777777779</v>
+        <v>29.555555555555557</v>
       </c>
       <c r="F2" s="0">
-        <v>29.777777777777779</v>
+        <v>29.555555555555557</v>
       </c>
       <c r="G2" s="0">
-        <v>29.777777777777779</v>
+        <v>29.555555555555557</v>
       </c>
       <c r="H2" s="0">
-        <v>29.777777777777779</v>
+        <v>29.555555555555557</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="B3" s="0">
-        <v>30.454545454545453</v>
+        <v>32.899999999999999</v>
       </c>
       <c r="C3" s="0">
-        <v>30.375</v>
+        <v>28.875</v>
       </c>
       <c r="D3" s="0">
-        <v>29.777777777777779</v>
+        <v>39.600000000000001</v>
       </c>
       <c r="E3" s="0">
-        <v>29.285714285714285</v>
+        <v>29.333333333333332</v>
       </c>
       <c r="F3" s="0">
-        <v>29.777777777777779</v>
+        <v>29.555555555555557</v>
       </c>
       <c r="G3" s="0">
-        <v>29.777777777777779</v>
+        <v>29.555555555555557</v>
       </c>
       <c r="H3" s="0">
-        <v>29.777777777777779</v>
+        <v>29.555555555555557</v>
       </c>
     </row>
   </sheetData>
@@ -593,99 +1029,290 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" customWidth="true"/>
-    <col min="2" max="2" width="12.21875" customWidth="true"/>
-    <col min="3" max="3" width="12.21875" customWidth="true"/>
-    <col min="4" max="4" width="12.21875" customWidth="true"/>
-    <col min="5" max="5" width="12.21875" customWidth="true"/>
-    <col min="6" max="6" width="12.21875" customWidth="true"/>
-    <col min="7" max="7" width="12.21875" customWidth="true"/>
-    <col min="8" max="8" width="12.21875" customWidth="true"/>
+    <col min="1" max="1" width="4.82421875" customWidth="true"/>
+    <col min="2" max="2" width="12.37890625" customWidth="true"/>
+    <col min="3" max="3" width="12.37890625" customWidth="true"/>
+    <col min="4" max="4" width="12.37890625" customWidth="true"/>
+    <col min="5" max="5" width="12.37890625" customWidth="true"/>
+    <col min="6" max="6" width="12.37890625" customWidth="true"/>
+    <col min="7" max="7" width="12.37890625" customWidth="true"/>
+    <col min="8" max="8" width="12.37890625" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>3</v>
+        <v>53</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="B2" s="0">
-        <v>-4159.932447906137</v>
+        <v>-4159.9324479061434</v>
       </c>
       <c r="C2" s="0">
         <v>-4159.9324479061434</v>
       </c>
       <c r="D2" s="0">
-        <v>-4159.9324479061388</v>
+        <v>-4159.9324479061497</v>
       </c>
       <c r="E2" s="0">
-        <v>-4159.9324479061388</v>
+        <v>-4159.9324479061488</v>
       </c>
       <c r="F2" s="0">
-        <v>-4159.9324479061388</v>
+        <v>-4159.9324479061488</v>
       </c>
       <c r="G2" s="0">
-        <v>-4159.9324479061388</v>
+        <v>-4159.9324479061488</v>
       </c>
       <c r="H2" s="0">
-        <v>-4159.9324479061388</v>
+        <v>-4159.9324479061488</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>2</v>
+        <v>52</v>
       </c>
       <c r="B3" s="0">
-        <v>-4159.9324479061434</v>
+        <v>-4159.9324479061397</v>
       </c>
       <c r="C3" s="0">
-        <v>-4159.9324479061434</v>
+        <v>-4159.9324479061415</v>
       </c>
       <c r="D3" s="0">
-        <v>-4159.9324479061452</v>
+        <v>-4159.932447906147</v>
       </c>
       <c r="E3" s="0">
+        <v>-4159.9324479061388</v>
+      </c>
+      <c r="F3" s="0">
         <v>-4159.9324479061488</v>
       </c>
+      <c r="G3" s="0">
+        <v>-4159.9324479061488</v>
+      </c>
+      <c r="H3" s="0">
+        <v>-4159.9324479061488</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="4.82421875" customWidth="true"/>
+    <col min="2" max="2" width="10.7109375" customWidth="true"/>
+    <col min="3" max="3" width="11.7109375" customWidth="true"/>
+    <col min="4" max="4" width="11.7109375" customWidth="true"/>
+    <col min="5" max="5" width="11.7109375" customWidth="true"/>
+    <col min="6" max="6" width="11.7109375" customWidth="true"/>
+    <col min="7" max="7" width="11.7109375" customWidth="true"/>
+    <col min="8" max="8" width="11.7109375" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="0">
+        <v>7.5658116900000012</v>
+      </c>
+      <c r="C2" s="0">
+        <v>4.1462608444444449</v>
+      </c>
+      <c r="D2" s="0">
+        <v>1.8907788222222217</v>
+      </c>
+      <c r="E2" s="0">
+        <v>10.78761489090909</v>
+      </c>
+      <c r="F2" s="0">
+        <v>10.866612036363636</v>
+      </c>
+      <c r="G2" s="0">
+        <v>10.846568872727273</v>
+      </c>
+      <c r="H2" s="0">
+        <v>10.731593818181819</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="0">
+        <v>29.785610411111104</v>
+      </c>
+      <c r="C3" s="0">
+        <v>7.852122145454544</v>
+      </c>
+      <c r="D3" s="0">
+        <v>7.3841942636363624</v>
+      </c>
+      <c r="E3" s="0">
+        <v>19.100514377777774</v>
+      </c>
       <c r="F3" s="0">
-        <v>-4159.9324479061388</v>
+        <v>23.231347427272727</v>
       </c>
       <c r="G3" s="0">
-        <v>-4159.9324479061388</v>
+        <v>23.200444118181817</v>
       </c>
       <c r="H3" s="0">
-        <v>-4159.9324479061388</v>
+        <v>10.731593818181819</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="4.82421875" customWidth="true"/>
+    <col min="2" max="2" width="6.82421875" customWidth="true"/>
+    <col min="3" max="3" width="11.7109375" customWidth="true"/>
+    <col min="4" max="4" width="11.7109375" customWidth="true"/>
+    <col min="5" max="5" width="11.7109375" customWidth="true"/>
+    <col min="6" max="6" width="11.7109375" customWidth="true"/>
+    <col min="7" max="7" width="11.7109375" customWidth="true"/>
+    <col min="8" max="8" width="11.7109375" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="0">
+        <v>87.900000000000006</v>
+      </c>
+      <c r="C2" s="0">
+        <v>64.222222222222229</v>
+      </c>
+      <c r="D2" s="0">
+        <v>46.111111111111114</v>
+      </c>
+      <c r="E2" s="0">
+        <v>112.63636363636364</v>
+      </c>
+      <c r="F2" s="0">
+        <v>112.63636363636364</v>
+      </c>
+      <c r="G2" s="0">
+        <v>112.63636363636364</v>
+      </c>
+      <c r="H2" s="0">
+        <v>112.63636363636364</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="0">
+        <v>138.11111111111111</v>
+      </c>
+      <c r="C3" s="0">
+        <v>50.727272727272727</v>
+      </c>
+      <c r="D3" s="0">
+        <v>48</v>
+      </c>
+      <c r="E3" s="0">
+        <v>96.555555555555557</v>
+      </c>
+      <c r="F3" s="0">
+        <v>112.63636363636364</v>
+      </c>
+      <c r="G3" s="0">
+        <v>112.63636363636364</v>
+      </c>
+      <c r="H3" s="0">
+        <v>112.63636363636364</v>
       </c>
     </row>
   </sheetData>

</xml_diff>